<commit_message>
Updated with new entries
</commit_message>
<xml_diff>
--- a/Signup_login.xlsx
+++ b/Signup_login.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Ecommerce_Manual_Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C46291EE-11E0-4418-9B73-511905822054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFAC724C-7AC5-4189-9A9C-D7D4EA59DCC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8B6476ED-93B3-458B-9892-B3A890F15F56}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="161">
   <si>
     <t>Product name</t>
   </si>
@@ -132,9 +132,6 @@
     <t>Functionality Testing</t>
   </si>
   <si>
-    <t>Verifing the logo is present in the footer section</t>
-  </si>
-  <si>
     <t>Signup and login</t>
   </si>
   <si>
@@ -463,6 +460,63 @@
   </si>
   <si>
     <t>Login operation should be run from different browser</t>
+  </si>
+  <si>
+    <t>It shouldn't take the empty field</t>
+  </si>
+  <si>
+    <t>It shouldn't take random numbers</t>
+  </si>
+  <si>
+    <t>Random alphabets shouldn't be taken</t>
+  </si>
+  <si>
+    <t>Shouldn't be taken the data without @</t>
+  </si>
+  <si>
+    <t>It shoudn't take the data with double @@</t>
+  </si>
+  <si>
+    <t>Every field should guide the user while filling up the fields</t>
+  </si>
+  <si>
+    <t>It should take the write information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sing up form should keep the data after attempting a wrong submission </t>
+  </si>
+  <si>
+    <t>there should be mendatory help icon for every field for the new user</t>
+  </si>
+  <si>
+    <t>Help icons should be connected to the correct field</t>
+  </si>
+  <si>
+    <t>There should be a persent of password field</t>
+  </si>
+  <si>
+    <t>Sign up submisssion shouldn't be successful if there any presence of space while entering the data</t>
+  </si>
+  <si>
+    <t>Signup up form should give specific error message for the specific problems</t>
+  </si>
+  <si>
+    <t>there should be verification mail</t>
+  </si>
+  <si>
+    <t>Mail should be verified by click on the link</t>
+  </si>
+  <si>
+    <t>There should be no submission if any user tries to sign up with same email address</t>
+  </si>
+  <si>
+    <t>Terms and policy and copy rights options should be present in the sign up form</t>
+  </si>
+  <si>
+    <t>There shouldn't be no submission with any username</t>
+  </si>
+  <si>
+    <t>Same data shouldn't be taken</t>
   </si>
 </sst>
 </file>
@@ -1236,8 +1290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA19025C-277F-4DBB-BB44-9F0A648F386E}">
   <dimension ref="A1:K143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="F142" sqref="F142:F143"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80:K80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1266,7 +1320,7 @@
         <v>5</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E1" s="28" t="s">
         <v>9</v>
@@ -1294,13 +1348,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="28" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E3" s="28" t="s">
         <v>10</v>
@@ -1454,19 +1508,19 @@
         <v>1</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>30</v>
       </c>
       <c r="D14" s="48" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
@@ -1495,10 +1549,10 @@
       <c r="C16" s="10"/>
       <c r="D16" s="49"/>
       <c r="E16" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
@@ -1527,10 +1581,10 @@
       <c r="C18" s="10"/>
       <c r="D18" s="49"/>
       <c r="E18" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G18" s="16"/>
       <c r="H18" s="16"/>
@@ -1559,10 +1613,10 @@
       <c r="C20" s="10"/>
       <c r="D20" s="49"/>
       <c r="E20" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G20" s="16"/>
       <c r="H20" s="16"/>
@@ -1591,10 +1645,10 @@
       <c r="C22" s="10"/>
       <c r="D22" s="49"/>
       <c r="E22" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G22" s="16"/>
       <c r="H22" s="16"/>
@@ -1623,10 +1677,10 @@
       <c r="C24" s="10"/>
       <c r="D24" s="49"/>
       <c r="E24" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G24" s="16"/>
       <c r="H24" s="16"/>
@@ -1655,10 +1709,10 @@
       <c r="C26" s="10"/>
       <c r="D26" s="49"/>
       <c r="E26" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G26" s="16"/>
       <c r="H26" s="16"/>
@@ -1687,10 +1741,10 @@
       <c r="C28" s="10"/>
       <c r="D28" s="49"/>
       <c r="E28" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G28" s="16"/>
       <c r="H28" s="16"/>
@@ -1719,10 +1773,10 @@
       <c r="C30" s="10"/>
       <c r="D30" s="49"/>
       <c r="E30" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G30" s="16"/>
       <c r="H30" s="16"/>
@@ -1751,10 +1805,10 @@
       <c r="C32" s="10"/>
       <c r="D32" s="49"/>
       <c r="E32" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G32" s="16"/>
       <c r="H32" s="16"/>
@@ -1783,10 +1837,10 @@
       <c r="C34" s="10"/>
       <c r="D34" s="49"/>
       <c r="E34" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G34" s="16"/>
       <c r="H34" s="3"/>
@@ -1853,16 +1907,18 @@
         <v>13</v>
       </c>
       <c r="B39" s="51" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C39" s="48" t="s">
         <v>31</v>
       </c>
       <c r="D39" s="49"/>
       <c r="E39" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="F39" s="9"/>
+        <v>55</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>142</v>
+      </c>
       <c r="G39" s="9"/>
       <c r="H39" s="9"/>
       <c r="I39" s="9"/>
@@ -1890,9 +1946,11 @@
       <c r="C41" s="49"/>
       <c r="D41" s="49"/>
       <c r="E41" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="F41" s="9"/>
+        <v>56</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>143</v>
+      </c>
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
       <c r="I41" s="9"/>
@@ -1920,9 +1978,11 @@
       <c r="C43" s="49"/>
       <c r="D43" s="49"/>
       <c r="E43" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="F43" s="9"/>
+        <v>57</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>144</v>
+      </c>
       <c r="G43" s="9"/>
       <c r="H43" s="9"/>
       <c r="I43" s="9"/>
@@ -1950,9 +2010,11 @@
       <c r="C45" s="49"/>
       <c r="D45" s="49"/>
       <c r="E45" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="F45" s="9"/>
+        <v>58</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>145</v>
+      </c>
       <c r="G45" s="9"/>
       <c r="H45" s="9"/>
       <c r="I45" s="9"/>
@@ -1980,9 +2042,11 @@
       <c r="C47" s="49"/>
       <c r="D47" s="49"/>
       <c r="E47" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="F47" s="9"/>
+        <v>59</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>146</v>
+      </c>
       <c r="G47" s="9"/>
       <c r="H47" s="9"/>
       <c r="I47" s="9"/>
@@ -2010,9 +2074,11 @@
       <c r="C49" s="49"/>
       <c r="D49" s="49"/>
       <c r="E49" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="F49" s="9"/>
+        <v>60</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>147</v>
+      </c>
       <c r="G49" s="9"/>
       <c r="H49" s="9"/>
       <c r="I49" s="9"/>
@@ -2040,9 +2106,11 @@
       <c r="C51" s="49"/>
       <c r="D51" s="49"/>
       <c r="E51" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="F51" s="9"/>
+        <v>61</v>
+      </c>
+      <c r="F51" s="9" t="s">
+        <v>148</v>
+      </c>
       <c r="G51" s="9"/>
       <c r="H51" s="9"/>
       <c r="I51" s="9"/>
@@ -2070,9 +2138,11 @@
       <c r="C53" s="49"/>
       <c r="D53" s="49"/>
       <c r="E53" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="F53" s="9"/>
+        <v>62</v>
+      </c>
+      <c r="F53" s="9" t="s">
+        <v>149</v>
+      </c>
       <c r="G53" s="9"/>
       <c r="H53" s="9"/>
       <c r="I53" s="9"/>
@@ -2100,9 +2170,11 @@
       <c r="C55" s="49"/>
       <c r="D55" s="49"/>
       <c r="E55" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F55" s="9"/>
+        <v>63</v>
+      </c>
+      <c r="F55" s="9" t="s">
+        <v>150</v>
+      </c>
       <c r="G55" s="9"/>
       <c r="H55" s="9"/>
       <c r="I55" s="9"/>
@@ -2130,9 +2202,11 @@
       <c r="C57" s="49"/>
       <c r="D57" s="49"/>
       <c r="E57" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="F57" s="9"/>
+        <v>64</v>
+      </c>
+      <c r="F57" s="9" t="s">
+        <v>151</v>
+      </c>
       <c r="G57" s="9"/>
       <c r="H57" s="9"/>
       <c r="I57" s="9"/>
@@ -2160,9 +2234,11 @@
       <c r="C59" s="49"/>
       <c r="D59" s="49"/>
       <c r="E59" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="F59" s="9"/>
+        <v>65</v>
+      </c>
+      <c r="F59" s="9" t="s">
+        <v>152</v>
+      </c>
       <c r="G59" s="9"/>
       <c r="H59" s="16"/>
       <c r="I59" s="16"/>
@@ -2190,9 +2266,11 @@
       <c r="C61" s="49"/>
       <c r="D61" s="49"/>
       <c r="E61" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="F61" s="31"/>
+        <v>66</v>
+      </c>
+      <c r="F61" s="31" t="s">
+        <v>153</v>
+      </c>
       <c r="G61" s="31"/>
       <c r="H61" s="31"/>
       <c r="I61" s="9"/>
@@ -2233,9 +2311,11 @@
       <c r="C64" s="49"/>
       <c r="D64" s="49"/>
       <c r="E64" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="F64" s="32"/>
+        <v>67</v>
+      </c>
+      <c r="F64" s="32" t="s">
+        <v>154</v>
+      </c>
       <c r="G64" s="32"/>
       <c r="H64" s="32"/>
       <c r="I64" s="32"/>
@@ -2263,9 +2343,11 @@
       <c r="C66" s="49"/>
       <c r="D66" s="49"/>
       <c r="E66" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="F66" s="9"/>
+        <v>68</v>
+      </c>
+      <c r="F66" s="9" t="s">
+        <v>155</v>
+      </c>
       <c r="G66" s="9"/>
       <c r="H66" s="9"/>
       <c r="I66" s="9"/>
@@ -2293,9 +2375,11 @@
       <c r="C68" s="49"/>
       <c r="D68" s="49"/>
       <c r="E68" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="F68" s="9"/>
+        <v>69</v>
+      </c>
+      <c r="F68" s="9" t="s">
+        <v>156</v>
+      </c>
       <c r="G68" s="9"/>
       <c r="H68" s="9"/>
       <c r="I68" s="9"/>
@@ -2323,9 +2407,11 @@
       <c r="C70" s="49"/>
       <c r="D70" s="49"/>
       <c r="E70" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="F70" s="9"/>
+        <v>70</v>
+      </c>
+      <c r="F70" s="9" t="s">
+        <v>157</v>
+      </c>
       <c r="G70" s="9"/>
       <c r="H70" s="9"/>
       <c r="I70" s="9"/>
@@ -2353,9 +2439,11 @@
       <c r="C72" s="49"/>
       <c r="D72" s="49"/>
       <c r="E72" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="F72" s="9"/>
+        <v>71</v>
+      </c>
+      <c r="F72" s="9" t="s">
+        <v>158</v>
+      </c>
       <c r="G72" s="9"/>
       <c r="H72" s="9"/>
       <c r="I72" s="9"/>
@@ -2383,9 +2471,11 @@
       <c r="C74" s="49"/>
       <c r="D74" s="49"/>
       <c r="E74" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="F74" s="9"/>
+        <v>72</v>
+      </c>
+      <c r="F74" s="9" t="s">
+        <v>159</v>
+      </c>
       <c r="G74" s="9"/>
       <c r="H74" s="9"/>
       <c r="I74" s="9"/>
@@ -2413,9 +2503,11 @@
       <c r="C76" s="49"/>
       <c r="D76" s="49"/>
       <c r="E76" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F76" s="9"/>
+        <v>73</v>
+      </c>
+      <c r="F76" s="9" t="s">
+        <v>160</v>
+      </c>
       <c r="G76" s="9"/>
       <c r="H76" s="9"/>
       <c r="I76" s="9"/>
@@ -2442,9 +2534,7 @@
       <c r="B78" s="52"/>
       <c r="C78" s="49"/>
       <c r="D78" s="49"/>
-      <c r="E78" s="9" t="s">
-        <v>32</v>
-      </c>
+      <c r="E78" s="9"/>
       <c r="F78" s="9"/>
       <c r="G78" s="9"/>
       <c r="H78" s="9"/>
@@ -2481,13 +2571,13 @@
     <row r="81" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C81" s="59" t="s">
         <v>79</v>
       </c>
-      <c r="C81" s="59" t="s">
+      <c r="D81" s="10" t="s">
         <v>80</v>
-      </c>
-      <c r="D81" s="10" t="s">
-        <v>81</v>
       </c>
       <c r="E81" s="60"/>
       <c r="F81" s="1"/>
@@ -2505,10 +2595,10 @@
       <c r="C82" s="59"/>
       <c r="D82" s="10"/>
       <c r="E82" s="43" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F82" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G82" s="9"/>
       <c r="H82" s="9"/>
@@ -2537,10 +2627,10 @@
       <c r="C84" s="59"/>
       <c r="D84" s="10"/>
       <c r="E84" s="43" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F84" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G84" s="16"/>
       <c r="H84" s="16"/>
@@ -2569,10 +2659,10 @@
       <c r="C86" s="59"/>
       <c r="D86" s="10"/>
       <c r="E86" s="43" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F86" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G86" s="9"/>
       <c r="H86" s="9"/>
@@ -2601,10 +2691,10 @@
       <c r="C88" s="59"/>
       <c r="D88" s="10"/>
       <c r="E88" s="43" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F88" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G88" s="9"/>
       <c r="H88" s="9"/>
@@ -2633,10 +2723,10 @@
       <c r="C90" s="59"/>
       <c r="D90" s="10"/>
       <c r="E90" s="43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F90" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G90" s="9"/>
       <c r="H90" s="9"/>
@@ -2665,10 +2755,10 @@
       <c r="C92" s="59"/>
       <c r="D92" s="10"/>
       <c r="E92" s="43" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F92" s="53" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G92" s="9"/>
       <c r="H92" s="9"/>
@@ -2709,10 +2799,10 @@
       <c r="C95" s="59"/>
       <c r="D95" s="10"/>
       <c r="E95" s="43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F95" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G95" s="9"/>
       <c r="H95" s="9"/>
@@ -2741,10 +2831,10 @@
       <c r="C97" s="59"/>
       <c r="D97" s="10"/>
       <c r="E97" s="43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F97" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G97" s="9"/>
       <c r="H97" s="9"/>
@@ -2773,10 +2863,10 @@
       <c r="C99" s="59"/>
       <c r="D99" s="10"/>
       <c r="E99" s="43" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F99" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G99" s="9"/>
       <c r="H99" s="9"/>
@@ -2805,10 +2895,10 @@
       <c r="C101" s="59"/>
       <c r="D101" s="10"/>
       <c r="E101" s="43" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F101" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G101" s="9"/>
       <c r="H101" s="9"/>
@@ -2837,10 +2927,10 @@
       <c r="C103" s="59"/>
       <c r="D103" s="10"/>
       <c r="E103" s="43" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F103" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G103" s="9"/>
       <c r="H103" s="9"/>
@@ -2869,10 +2959,10 @@
       <c r="C105" s="59"/>
       <c r="D105" s="10"/>
       <c r="E105" s="43" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F105" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G105" s="9"/>
       <c r="H105" s="9"/>
@@ -2901,10 +2991,10 @@
       <c r="C107" s="59"/>
       <c r="D107" s="10"/>
       <c r="E107" s="43" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F107" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G107" s="9"/>
       <c r="H107" s="9"/>
@@ -2933,10 +3023,10 @@
       <c r="C109" s="59"/>
       <c r="D109" s="10"/>
       <c r="E109" s="43" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F109" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G109" s="9"/>
       <c r="H109" s="9"/>
@@ -2965,10 +3055,10 @@
       <c r="C111" s="59"/>
       <c r="D111" s="10"/>
       <c r="E111" s="43" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F111" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G111" s="9"/>
       <c r="H111" s="9"/>
@@ -2997,7 +3087,7 @@
       <c r="C113" s="59"/>
       <c r="D113" s="10"/>
       <c r="E113" s="43" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F113" s="9"/>
       <c r="G113" s="9"/>
@@ -3035,17 +3125,17 @@
     <row r="116" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="29"/>
       <c r="B116" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="C116" s="10" t="s">
         <v>112</v>
-      </c>
-      <c r="C116" s="10" t="s">
-        <v>113</v>
       </c>
       <c r="D116" s="10"/>
       <c r="E116" s="43" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F116" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="117" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3062,10 +3152,10 @@
       <c r="C118" s="10"/>
       <c r="D118" s="10"/>
       <c r="E118" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F118" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="119" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3082,10 +3172,10 @@
       <c r="C120" s="10"/>
       <c r="D120" s="10"/>
       <c r="E120" s="43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F120" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="121" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3102,10 +3192,10 @@
       <c r="C122" s="10"/>
       <c r="D122" s="10"/>
       <c r="E122" s="43" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F122" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="123" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3122,10 +3212,10 @@
       <c r="C124" s="10"/>
       <c r="D124" s="10"/>
       <c r="E124" s="43" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F124" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="125" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3142,10 +3232,10 @@
       <c r="C126" s="10"/>
       <c r="D126" s="10"/>
       <c r="E126" s="43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F126" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="127" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3162,10 +3252,10 @@
       <c r="C128" s="10"/>
       <c r="D128" s="10"/>
       <c r="E128" s="43" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F128" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="129" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3182,10 +3272,10 @@
       <c r="C130" s="10"/>
       <c r="D130" s="10"/>
       <c r="E130" s="43" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F130" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="131" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3202,10 +3292,10 @@
       <c r="C132" s="10"/>
       <c r="D132" s="10"/>
       <c r="E132" s="43" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F132" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="133" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3222,10 +3312,10 @@
       <c r="C134" s="10"/>
       <c r="D134" s="10"/>
       <c r="E134" s="43" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F134" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="135" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3242,10 +3332,10 @@
       <c r="C136" s="10"/>
       <c r="D136" s="10"/>
       <c r="E136" s="43" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F136" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="137" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3262,10 +3352,10 @@
       <c r="C138" s="10"/>
       <c r="D138" s="10"/>
       <c r="E138" s="43" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F138" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="139" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3282,10 +3372,10 @@
       <c r="C140" s="10"/>
       <c r="D140" s="10"/>
       <c r="E140" s="43" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F140" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="141" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3302,10 +3392,10 @@
       <c r="C142" s="10"/>
       <c r="D142" s="10"/>
       <c r="E142" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F142" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>